<commit_message>
Asignación de recursos Mat 8 tema 3
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1235,9 +1235,6 @@
     <t>Cristhian</t>
   </si>
   <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
     <t>Josué</t>
   </si>
   <si>
@@ -1245,6 +1242,9 @@
   </si>
   <si>
     <t>Solicitud gráfica enviada el 7/09/2015</t>
+  </si>
+  <si>
+    <t>Adriana</t>
   </si>
 </sst>
 </file>
@@ -1725,18 +1725,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1775,6 +1763,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6368,7 +6368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1085"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
@@ -6401,81 +6401,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="37" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="104" t="s">
         <v>357</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="106" t="s">
         <v>358</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="108" t="s">
         <v>359</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="H1" s="108" t="s">
         <v>360</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="108" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="105" t="s">
+      <c r="J1" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="104" t="s">
+      <c r="K1" s="100" t="s">
         <v>355</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="L1" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="106"/>
+      <c r="N1" s="102"/>
       <c r="O1" s="96" t="s">
         <v>197</v>
       </c>
       <c r="P1" s="96" t="s">
         <v>356</v>
       </c>
-      <c r="Q1" s="100" t="s">
+      <c r="Q1" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="99" t="s">
+      <c r="R1" s="112" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="97" t="s">
+      <c r="S1" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="98" t="s">
+      <c r="T1" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="U1" s="97" t="s">
+      <c r="U1" s="110" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="37" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="103"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="99"/>
       <c r="M2" s="48" t="s">
         <v>124</v>
       </c>
@@ -6484,11 +6484,11 @@
       </c>
       <c r="O2" s="96"/>
       <c r="P2" s="96"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="97"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="110"/>
     </row>
     <row r="3" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
@@ -6545,10 +6545,10 @@
         <v>282</v>
       </c>
       <c r="V3" s="62" t="s">
+        <v>365</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>366</v>
-      </c>
-      <c r="W3" s="37" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6741,7 +6741,7 @@
         <v>364</v>
       </c>
       <c r="W6" s="35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:23" s="80" customFormat="1" x14ac:dyDescent="0.25">
@@ -6801,7 +6801,7 @@
         <v>282</v>
       </c>
       <c r="V7" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -6868,7 +6868,7 @@
         <v>364</v>
       </c>
       <c r="W8" s="35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -6935,7 +6935,7 @@
         <v>364</v>
       </c>
       <c r="W9" s="35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="71" customFormat="1" x14ac:dyDescent="0.25">
@@ -6995,7 +6995,7 @@
         <v>349</v>
       </c>
       <c r="V10" s="70" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -7187,7 +7187,7 @@
         <v>310</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -7251,7 +7251,7 @@
         <v>310</v>
       </c>
       <c r="V14" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -7315,7 +7315,7 @@
         <v>310</v>
       </c>
       <c r="V15" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -7379,7 +7379,7 @@
         <v>301</v>
       </c>
       <c r="V16" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -7443,7 +7443,7 @@
         <v>310</v>
       </c>
       <c r="V17" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -7507,7 +7507,7 @@
         <v>310</v>
       </c>
       <c r="V18" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="71" customFormat="1" x14ac:dyDescent="0.25">
@@ -7567,7 +7567,7 @@
         <v>353</v>
       </c>
       <c r="V19" s="70" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -7631,7 +7631,7 @@
         <v>310</v>
       </c>
       <c r="V20" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -7821,7 +7821,7 @@
         <v>310</v>
       </c>
       <c r="V23" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -7885,7 +7885,7 @@
         <v>310</v>
       </c>
       <c r="V24" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -7947,7 +7947,7 @@
         <v>301</v>
       </c>
       <c r="V25" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -8071,7 +8071,7 @@
         <v>301</v>
       </c>
       <c r="V27" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -8135,7 +8135,7 @@
         <v>310</v>
       </c>
       <c r="V28" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -8199,7 +8199,7 @@
         <v>310</v>
       </c>
       <c r="V29" s="59" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -8321,7 +8321,7 @@
         <v>282</v>
       </c>
       <c r="V31" s="70" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -12351,6 +12351,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -12365,12 +12371,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K35">

</xml_diff>

<commit_message>
cambio nombre recursos tema 3 grado 8 matemáticas
Se actualiza la escaleta por el cambio de nombre de dos recursos en
GRECO.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\grado08\guion03\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7215" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -686,9 +681,6 @@
     <t>Los cocientes notables</t>
   </si>
   <si>
-    <t>Competencias: expresiones algebraicas que representan áreas</t>
-  </si>
-  <si>
     <t>Actividad que permite relacionar expresiones algebraicas con áreas de diferentes figuras</t>
   </si>
   <si>
@@ -813,9 +805,6 @@
   </si>
   <si>
     <t>MT</t>
-  </si>
-  <si>
-    <t>Competencias: las identidades notables</t>
   </si>
   <si>
     <t>Actividad uqe permite argumentar sobre características de las identidades notables</t>
@@ -1333,6 +1322,12 @@
   </si>
   <si>
     <t>envíar para que lo suba Pedro</t>
+  </si>
+  <si>
+    <t>Las identidades notables</t>
+  </si>
+  <si>
+    <t>Expresiones algebraicas que representan áreas</t>
   </si>
 </sst>
 </file>
@@ -1731,8 +1726,33 @@
     <xf numFmtId="14" fontId="7" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1772,31 +1792,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1858,7 +1853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1893,7 +1888,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6390,8 +6385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR1085"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6425,99 +6420,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="32" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="71" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="G1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="75" t="s">
         <v>342</v>
       </c>
-      <c r="F1" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="66" t="s">
-        <v>344</v>
-      </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="58" t="s">
-        <v>339</v>
-      </c>
-      <c r="L1" s="57" t="s">
+      <c r="K1" s="67" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="54" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="54" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q1" s="71" t="s">
+      <c r="P1" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q1" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="70" t="s">
+      <c r="R1" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="68" t="s">
+      <c r="S1" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="60" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="57"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="33" t="s">
         <v>124</v>
       </c>
       <c r="N2" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="68"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="60"/>
       <c r="W2" s="40" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="X2" s="37" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:44" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -6535,17 +6530,17 @@
       </c>
       <c r="E3" s="46"/>
       <c r="F3" s="46"/>
-      <c r="G3" s="72" t="s">
-        <v>318</v>
+      <c r="G3" s="54" t="s">
+        <v>316</v>
       </c>
       <c r="H3" s="46">
         <v>1</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="55" t="s">
         <v>204</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K3" s="42" t="s">
         <v>204</v>
@@ -6557,28 +6552,28 @@
       <c r="N3" s="42"/>
       <c r="O3" s="43"/>
       <c r="P3" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q3" s="74" t="s">
-        <v>329</v>
-      </c>
-      <c r="R3" s="74" t="s">
-        <v>263</v>
-      </c>
-      <c r="S3" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="R3" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="S3" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="T3" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="U3" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T3" s="74" t="s">
-        <v>274</v>
-      </c>
-      <c r="U3" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="V3" s="75" t="s">
-        <v>349</v>
-      </c>
-      <c r="W3" s="75" t="s">
-        <v>362</v>
+      <c r="V3" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="W3" s="57" t="s">
+        <v>360</v>
       </c>
       <c r="X3" s="51">
         <v>42294</v>
@@ -6599,17 +6594,17 @@
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
-      <c r="G4" s="72" t="s">
-        <v>223</v>
+      <c r="G4" s="54" t="s">
+        <v>222</v>
       </c>
       <c r="H4" s="46">
         <v>2</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="55" t="s">
         <v>205</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>205</v>
@@ -6622,7 +6617,7 @@
         <v>105</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P4" s="47" t="s">
         <v>205</v>
@@ -6631,28 +6626,28 @@
         <v>6</v>
       </c>
       <c r="R4" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="S4" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T4" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="U4" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T4" s="48" t="s">
-        <v>295</v>
-      </c>
-      <c r="U4" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V4" s="75" t="s">
-        <v>348</v>
-      </c>
-      <c r="W4" s="75" t="s">
-        <v>362</v>
+      <c r="V4" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="W4" s="57" t="s">
+        <v>360</v>
       </c>
       <c r="X4" s="51">
         <v>42294</v>
       </c>
       <c r="Y4" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
@@ -6673,7 +6668,7 @@
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H5" s="42">
         <v>3</v>
@@ -6682,7 +6677,7 @@
         <v>205</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K5" s="42" t="s">
         <v>205</v>
@@ -6695,31 +6690,31 @@
         <v>127</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P5" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q5" s="48">
         <v>6</v>
       </c>
       <c r="R5" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S5" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T5" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="U5" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T5" s="48" t="s">
-        <v>297</v>
-      </c>
-      <c r="U5" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V5" s="75" t="s">
-        <v>348</v>
+      <c r="V5" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W5" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X5" s="51">
         <v>42294</v>
@@ -6743,7 +6738,7 @@
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H6" s="46">
         <v>4</v>
@@ -6752,7 +6747,7 @@
         <v>205</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>205</v>
@@ -6765,7 +6760,7 @@
         <v>138</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P6" s="47" t="s">
         <v>205</v>
@@ -6774,28 +6769,28 @@
         <v>6</v>
       </c>
       <c r="R6" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S6" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T6" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="U6" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T6" s="48" t="s">
-        <v>298</v>
-      </c>
-      <c r="U6" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V6" s="75" t="s">
-        <v>348</v>
+      <c r="V6" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W6" s="41" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X6" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y6" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:44" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -6816,7 +6811,7 @@
       </c>
       <c r="F7" s="45"/>
       <c r="G7" s="43" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H7" s="46">
         <v>5</v>
@@ -6825,7 +6820,7 @@
         <v>205</v>
       </c>
       <c r="J7" s="45" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K7" s="42" t="s">
         <v>204</v>
@@ -6840,28 +6835,28 @@
         <v>205</v>
       </c>
       <c r="Q7" s="48" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="R7" s="48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="S7" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="T7" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="U7" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="T7" s="48" t="s">
-        <v>273</v>
-      </c>
-      <c r="U7" s="48" t="s">
-        <v>269</v>
-      </c>
-      <c r="V7" s="75" t="s">
-        <v>349</v>
+      <c r="V7" s="57" t="s">
+        <v>347</v>
       </c>
       <c r="W7" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X7" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y7" s="35"/>
       <c r="Z7" s="35"/>
@@ -6902,7 +6897,7 @@
       </c>
       <c r="F8" s="45"/>
       <c r="G8" s="43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H8" s="46">
         <v>6</v>
@@ -6911,7 +6906,7 @@
         <v>205</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>205</v>
@@ -6924,34 +6919,34 @@
         <v>138</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P8" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q8" s="48">
         <v>6</v>
       </c>
       <c r="R8" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S8" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T8" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="U8" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T8" s="48" t="s">
-        <v>299</v>
-      </c>
-      <c r="U8" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V8" s="75" t="s">
-        <v>348</v>
+      <c r="V8" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W8" s="50">
         <v>42254</v>
       </c>
       <c r="X8" s="53" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
@@ -6968,11 +6963,11 @@
         <v>209</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="43" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H9" s="46">
         <v>7</v>
@@ -6981,7 +6976,7 @@
         <v>205</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>205</v>
@@ -6994,37 +6989,37 @@
         <v>138</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q9" s="48">
         <v>6</v>
       </c>
       <c r="R9" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S9" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T9" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="U9" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T9" s="48" t="s">
-        <v>301</v>
-      </c>
-      <c r="U9" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V9" s="75" t="s">
-        <v>348</v>
+      <c r="V9" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W9" s="41" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X9" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y9" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:44" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -7041,11 +7036,11 @@
         <v>209</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F10" s="45"/>
       <c r="G10" s="43" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H10" s="46">
         <v>8</v>
@@ -7054,7 +7049,7 @@
         <v>205</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K10" s="42" t="s">
         <v>204</v>
@@ -7066,31 +7061,31 @@
       <c r="N10" s="42"/>
       <c r="O10" s="45"/>
       <c r="P10" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q10" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q10" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="R10" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="S10" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="T10" s="56" t="s">
         <v>330</v>
       </c>
-      <c r="R10" s="74" t="s">
-        <v>263</v>
-      </c>
-      <c r="S10" s="74" t="s">
+      <c r="U10" s="56" t="s">
         <v>331</v>
       </c>
-      <c r="T10" s="74" t="s">
-        <v>332</v>
-      </c>
-      <c r="U10" s="74" t="s">
-        <v>333</v>
-      </c>
-      <c r="V10" s="75" t="s">
-        <v>349</v>
+      <c r="V10" s="57" t="s">
+        <v>347</v>
       </c>
       <c r="W10" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X10" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y10" s="35"/>
       <c r="Z10" s="35"/>
@@ -7127,11 +7122,11 @@
         <v>209</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F11" s="45"/>
       <c r="G11" s="43" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H11" s="46">
         <v>9</v>
@@ -7140,7 +7135,7 @@
         <v>205</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>205</v>
@@ -7153,37 +7148,37 @@
         <v>137</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P11" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q11" s="48">
         <v>6</v>
       </c>
       <c r="R11" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S11" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T11" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="U11" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T11" s="48" t="s">
-        <v>302</v>
-      </c>
-      <c r="U11" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="V11" s="75" t="s">
-        <v>348</v>
+      <c r="V11" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W11" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X11" s="52">
         <v>42294</v>
       </c>
       <c r="Y11" s="30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
@@ -7204,7 +7199,7 @@
       </c>
       <c r="F12" s="45"/>
       <c r="G12" s="43" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H12" s="46">
         <v>10</v>
@@ -7213,7 +7208,7 @@
         <v>204</v>
       </c>
       <c r="J12" s="45" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>205</v>
@@ -7226,37 +7221,37 @@
       </c>
       <c r="N12" s="42"/>
       <c r="O12" s="45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P12" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q12" s="48">
         <v>6</v>
       </c>
       <c r="R12" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="S12" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T12" s="48" t="s">
         <v>284</v>
       </c>
-      <c r="S12" s="48" t="s">
+      <c r="U12" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T12" s="48" t="s">
-        <v>286</v>
-      </c>
-      <c r="U12" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="V12" s="75" t="s">
-        <v>348</v>
+      <c r="V12" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W12" s="41" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="X12" s="53">
         <v>42297</v>
       </c>
       <c r="Y12" s="30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -7277,7 +7272,7 @@
       </c>
       <c r="F13" s="45"/>
       <c r="G13" s="43" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H13" s="46">
         <v>11</v>
@@ -7286,7 +7281,7 @@
         <v>205</v>
       </c>
       <c r="J13" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K13" s="42" t="s">
         <v>205</v>
@@ -7299,34 +7294,34 @@
         <v>137</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P13" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q13" s="48">
         <v>6</v>
       </c>
       <c r="R13" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S13" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T13" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="U13" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T13" s="48" t="s">
-        <v>303</v>
-      </c>
-      <c r="U13" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V13" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W13" s="35" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="X13" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
@@ -7369,34 +7364,34 @@
         <v>127</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P14" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q14" s="48">
         <v>6</v>
       </c>
       <c r="R14" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S14" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T14" s="48" t="s">
+        <v>302</v>
+      </c>
+      <c r="U14" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T14" s="48" t="s">
-        <v>304</v>
-      </c>
-      <c r="U14" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V14" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W14" s="35" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="X14" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
@@ -7417,7 +7412,7 @@
       </c>
       <c r="F15" s="45"/>
       <c r="G15" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H15" s="46">
         <v>13</v>
@@ -7426,7 +7421,7 @@
         <v>205</v>
       </c>
       <c r="J15" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K15" s="42" t="s">
         <v>205</v>
@@ -7439,7 +7434,7 @@
         <v>138</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P15" s="47" t="s">
         <v>205</v>
@@ -7448,22 +7443,22 @@
         <v>6</v>
       </c>
       <c r="R15" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S15" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T15" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="U15" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T15" s="48" t="s">
-        <v>305</v>
-      </c>
-      <c r="U15" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V15" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W15" s="41" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="X15" s="53">
         <v>42297</v>
@@ -7496,7 +7491,7 @@
         <v>204</v>
       </c>
       <c r="J16" s="45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K16" s="42" t="s">
         <v>205</v>
@@ -7509,31 +7504,31 @@
       </c>
       <c r="N16" s="42"/>
       <c r="O16" s="45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P16" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q16" s="48">
         <v>6</v>
       </c>
       <c r="R16" s="48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S16" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T16" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="U16" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T16" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="U16" s="48" t="s">
-        <v>287</v>
-      </c>
       <c r="V16" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W16" s="41" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="X16" s="53">
         <v>42297</v>
@@ -7557,7 +7552,7 @@
       </c>
       <c r="F17" s="45"/>
       <c r="G17" s="43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H17" s="42">
         <v>15</v>
@@ -7566,7 +7561,7 @@
         <v>205</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K17" s="42" t="s">
         <v>205</v>
@@ -7579,7 +7574,7 @@
         <v>99</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P17" s="47" t="s">
         <v>205</v>
@@ -7588,25 +7583,25 @@
         <v>6</v>
       </c>
       <c r="R17" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S17" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T17" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="U17" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T17" s="48" t="s">
-        <v>347</v>
-      </c>
-      <c r="U17" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V17" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W17" s="50">
         <v>42292</v>
       </c>
       <c r="X17" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
@@ -7627,7 +7622,7 @@
       </c>
       <c r="F18" s="45"/>
       <c r="G18" s="43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H18" s="46">
         <v>16</v>
@@ -7636,7 +7631,7 @@
         <v>205</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K18" s="42" t="s">
         <v>205</v>
@@ -7649,34 +7644,34 @@
         <v>127</v>
       </c>
       <c r="O18" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P18" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q18" s="48">
         <v>6</v>
       </c>
       <c r="R18" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S18" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T18" s="48" t="s">
+        <v>308</v>
+      </c>
+      <c r="U18" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T18" s="48" t="s">
-        <v>310</v>
-      </c>
-      <c r="U18" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V18" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W18" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X18" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:39" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -7697,7 +7692,7 @@
       </c>
       <c r="F19" s="45"/>
       <c r="G19" s="43" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H19" s="42">
         <v>17</v>
@@ -7706,7 +7701,7 @@
         <v>205</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K19" s="42" t="s">
         <v>204</v>
@@ -7720,31 +7715,31 @@
       </c>
       <c r="O19" s="45"/>
       <c r="P19" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q19" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q19" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="R19" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="S19" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="T19" s="56" t="s">
         <v>334</v>
       </c>
-      <c r="R19" s="74" t="s">
-        <v>263</v>
-      </c>
-      <c r="S19" s="74" t="s">
+      <c r="U19" s="56" t="s">
         <v>335</v>
       </c>
-      <c r="T19" s="74" t="s">
-        <v>336</v>
-      </c>
-      <c r="U19" s="74" t="s">
-        <v>337</v>
-      </c>
-      <c r="V19" s="75" t="s">
-        <v>349</v>
+      <c r="V19" s="57" t="s">
+        <v>347</v>
       </c>
       <c r="W19" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X19" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y19" s="35"/>
       <c r="Z19" s="35"/>
@@ -7779,7 +7774,7 @@
       </c>
       <c r="F20" s="45"/>
       <c r="G20" s="43" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H20" s="42">
         <v>18</v>
@@ -7788,7 +7783,7 @@
         <v>205</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K20" s="42" t="s">
         <v>205</v>
@@ -7801,7 +7796,7 @@
         <v>116</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P20" s="47" t="s">
         <v>205</v>
@@ -7810,28 +7805,28 @@
         <v>6</v>
       </c>
       <c r="R20" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S20" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T20" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="U20" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T20" s="48" t="s">
-        <v>300</v>
-      </c>
-      <c r="U20" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V20" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W20" s="41" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="X20" s="53">
         <v>42297</v>
       </c>
       <c r="Y20" s="30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
@@ -7859,7 +7854,7 @@
         <v>204</v>
       </c>
       <c r="J21" s="45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K21" s="42" t="s">
         <v>205</v>
@@ -7872,28 +7867,28 @@
       </c>
       <c r="N21" s="42"/>
       <c r="O21" s="45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P21" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q21" s="48">
         <v>6</v>
       </c>
       <c r="R21" s="48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S21" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T21" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="U21" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T21" s="48" t="s">
-        <v>290</v>
-      </c>
-      <c r="U21" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="V21" s="75" t="s">
-        <v>348</v>
+      <c r="V21" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W21" s="50">
         <v>42297</v>
@@ -7902,7 +7897,7 @@
         <v>42299</v>
       </c>
       <c r="Y21" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -7932,7 +7927,7 @@
         <v>204</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K22" s="42" t="s">
         <v>205</v>
@@ -7945,28 +7940,28 @@
       </c>
       <c r="N22" s="42"/>
       <c r="O22" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P22" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q22" s="48">
         <v>6</v>
       </c>
       <c r="R22" s="48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S22" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T22" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="U22" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T22" s="48" t="s">
-        <v>292</v>
-      </c>
-      <c r="U22" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="V22" s="75" t="s">
-        <v>348</v>
+      <c r="V22" s="57" t="s">
+        <v>346</v>
       </c>
       <c r="W22" s="50">
         <v>42294</v>
@@ -7993,7 +7988,7 @@
       </c>
       <c r="F23" s="45"/>
       <c r="G23" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H23" s="46">
         <v>21</v>
@@ -8002,7 +7997,7 @@
         <v>205</v>
       </c>
       <c r="J23" s="45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K23" s="42" t="s">
         <v>205</v>
@@ -8015,37 +8010,37 @@
         <v>137</v>
       </c>
       <c r="O23" s="45" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P23" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q23" s="48">
         <v>6</v>
       </c>
       <c r="R23" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S23" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T23" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="U23" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T23" s="48" t="s">
-        <v>311</v>
-      </c>
-      <c r="U23" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V23" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X23" s="50">
         <v>42297</v>
       </c>
       <c r="Y23" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
@@ -8066,7 +8061,7 @@
       </c>
       <c r="F24" s="45"/>
       <c r="G24" s="43" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H24" s="42">
         <v>22</v>
@@ -8088,34 +8083,34 @@
         <v>116</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P24" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q24" s="48">
         <v>6</v>
       </c>
       <c r="R24" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S24" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T24" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="U24" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T24" s="48" t="s">
-        <v>306</v>
-      </c>
-      <c r="U24" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V24" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W24" s="50">
         <v>42294</v>
       </c>
       <c r="X24" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
@@ -8143,7 +8138,7 @@
         <v>204</v>
       </c>
       <c r="J25" s="45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K25" s="42" t="s">
         <v>205</v>
@@ -8156,34 +8151,34 @@
       </c>
       <c r="N25" s="42"/>
       <c r="O25" s="45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P25" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q25" s="48">
         <v>6</v>
       </c>
       <c r="R25" s="48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S25" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T25" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="U25" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T25" s="48" t="s">
-        <v>289</v>
-      </c>
-      <c r="U25" s="48" t="s">
-        <v>287</v>
-      </c>
       <c r="V25" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W25" s="50">
         <v>42299</v>
       </c>
-      <c r="X25" s="76" t="s">
-        <v>361</v>
+      <c r="X25" s="58" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
@@ -8202,7 +8197,7 @@
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
       <c r="G26" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H26" s="46">
         <v>24</v>
@@ -8211,7 +8206,7 @@
         <v>205</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K26" s="42" t="s">
         <v>205</v>
@@ -8224,37 +8219,37 @@
         <v>101</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="P26" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q26" s="48">
         <v>6</v>
       </c>
       <c r="R26" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S26" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T26" s="48" t="s">
+        <v>343</v>
+      </c>
+      <c r="U26" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T26" s="48" t="s">
-        <v>345</v>
-      </c>
-      <c r="U26" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V26" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W26" s="41" t="s">
-        <v>358</v>
-      </c>
-      <c r="X26" s="76" t="s">
-        <v>370</v>
+        <v>356</v>
+      </c>
+      <c r="X26" s="58" t="s">
+        <v>368</v>
       </c>
       <c r="Y26" s="30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -8273,7 +8268,7 @@
       <c r="E27" s="45"/>
       <c r="F27" s="45"/>
       <c r="G27" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H27" s="46">
         <v>25</v>
@@ -8282,7 +8277,7 @@
         <v>204</v>
       </c>
       <c r="J27" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K27" s="42" t="s">
         <v>205</v>
@@ -8295,37 +8290,37 @@
       </c>
       <c r="N27" s="42"/>
       <c r="O27" s="45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P27" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q27" s="48">
         <v>6</v>
       </c>
       <c r="R27" s="48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S27" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="T27" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="U27" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T27" s="48" t="s">
-        <v>291</v>
-      </c>
-      <c r="U27" s="48" t="s">
-        <v>287</v>
-      </c>
       <c r="V27" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W27" s="41" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="X27" s="53">
         <v>42297</v>
       </c>
       <c r="Y27" s="49" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
@@ -8346,7 +8341,7 @@
       </c>
       <c r="F28" s="45"/>
       <c r="G28" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H28" s="46">
         <v>26</v>
@@ -8355,7 +8350,7 @@
         <v>205</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K28" s="42" t="s">
         <v>205</v>
@@ -8368,31 +8363,31 @@
         <v>116</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q28" s="48">
         <v>6</v>
       </c>
       <c r="R28" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S28" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T28" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="U28" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T28" s="48" t="s">
-        <v>307</v>
-      </c>
-      <c r="U28" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V28" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W28" s="41" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="X28" s="53">
         <v>42297</v>
@@ -8416,7 +8411,7 @@
       </c>
       <c r="F29" s="45"/>
       <c r="G29" s="43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H29" s="46">
         <v>27</v>
@@ -8425,7 +8420,7 @@
         <v>205</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="K29" s="42" t="s">
         <v>205</v>
@@ -8438,7 +8433,7 @@
         <v>116</v>
       </c>
       <c r="O29" s="45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P29" s="47" t="s">
         <v>205</v>
@@ -8447,19 +8442,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S29" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T29" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="U29" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T29" s="48" t="s">
-        <v>308</v>
-      </c>
-      <c r="U29" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V29" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="W29" s="50">
         <v>42290</v>
@@ -8484,7 +8479,7 @@
       <c r="E30" s="45"/>
       <c r="F30" s="45"/>
       <c r="G30" s="43" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H30" s="46">
         <v>28</v>
@@ -8493,7 +8488,7 @@
         <v>205</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K30" s="42" t="s">
         <v>205</v>
@@ -8506,34 +8501,34 @@
         <v>118</v>
       </c>
       <c r="O30" s="45" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P30" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q30" s="48">
         <v>6</v>
       </c>
       <c r="R30" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S30" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T30" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="U30" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T30" s="48" t="s">
-        <v>309</v>
-      </c>
-      <c r="U30" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V30" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W30" s="50">
         <v>42303</v>
       </c>
-      <c r="X30" s="76" t="s">
-        <v>361</v>
+      <c r="X30" s="58" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="1:39" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -8552,7 +8547,7 @@
       <c r="E31" s="45"/>
       <c r="F31" s="45"/>
       <c r="G31" s="43" t="s">
-        <v>264</v>
+        <v>385</v>
       </c>
       <c r="H31" s="46">
         <v>29</v>
@@ -8561,7 +8556,7 @@
         <v>205</v>
       </c>
       <c r="J31" s="45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K31" s="42" t="s">
         <v>204</v>
@@ -8574,34 +8569,34 @@
         <v>116</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P31" s="47" t="s">
         <v>205</v>
       </c>
       <c r="Q31" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="R31" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="S31" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="T31" s="48" t="s">
         <v>266</v>
       </c>
-      <c r="R31" s="48" t="s">
-        <v>263</v>
-      </c>
-      <c r="S31" s="48" t="s">
+      <c r="U31" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="T31" s="48" t="s">
-        <v>268</v>
-      </c>
-      <c r="U31" s="48" t="s">
-        <v>269</v>
-      </c>
-      <c r="V31" s="75" t="s">
-        <v>349</v>
+      <c r="V31" s="57" t="s">
+        <v>347</v>
       </c>
       <c r="W31" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X31" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y31" s="35"/>
       <c r="Z31" s="35"/>
@@ -8635,7 +8630,7 @@
       <c r="E32" s="45"/>
       <c r="F32" s="45"/>
       <c r="G32" s="43" t="s">
-        <v>221</v>
+        <v>386</v>
       </c>
       <c r="H32" s="46">
         <v>30</v>
@@ -8644,7 +8639,7 @@
         <v>205</v>
       </c>
       <c r="J32" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K32" s="42" t="s">
         <v>205</v>
@@ -8657,7 +8652,7 @@
         <v>138</v>
       </c>
       <c r="O32" s="45" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P32" s="47" t="s">
         <v>205</v>
@@ -8666,25 +8661,25 @@
         <v>6</v>
       </c>
       <c r="R32" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S32" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T32" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="U32" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T32" s="48" t="s">
-        <v>313</v>
-      </c>
-      <c r="U32" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V32" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W32" s="50">
         <v>42297</v>
       </c>
-      <c r="X32" s="76" t="s">
-        <v>361</v>
+      <c r="X32" s="58" t="s">
+        <v>359</v>
       </c>
       <c r="Y32" s="35"/>
       <c r="Z32" s="35"/>
@@ -8713,7 +8708,7 @@
         <v>208</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E33" s="45"/>
       <c r="F33" s="45"/>
@@ -8740,7 +8735,7 @@
       <c r="U33" s="45"/>
       <c r="V33" s="35"/>
       <c r="W33" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X33" s="53">
         <v>42297</v>
@@ -8757,12 +8752,12 @@
         <v>208</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="43" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H34" s="46">
         <v>32</v>
@@ -8771,7 +8766,7 @@
         <v>205</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K34" s="42" t="s">
         <v>205</v>
@@ -8791,25 +8786,25 @@
         <v>6</v>
       </c>
       <c r="R34" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S34" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="T34" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="U34" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="T34" s="48" t="s">
-        <v>312</v>
-      </c>
-      <c r="U34" s="48" t="s">
-        <v>296</v>
-      </c>
       <c r="V34" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W34" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="X34" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
@@ -8823,10 +8818,10 @@
         <v>208</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E35" s="45" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F35" s="45"/>
       <c r="G35" s="43"/>
@@ -8851,7 +8846,7 @@
       <c r="T35" s="45"/>
       <c r="U35" s="45"/>
       <c r="V35" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W35" s="50">
         <v>42296</v>
@@ -8860,7 +8855,7 @@
         <v>42297</v>
       </c>
       <c r="Y35" s="49" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -8923,7 +8918,7 @@
         <v>21</v>
       </c>
       <c r="Q39" s="36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -8939,7 +8934,7 @@
         <v>9</v>
       </c>
       <c r="Q40" s="36" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -12689,12 +12684,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -12709,6 +12698,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K35">

</xml_diff>

<commit_message>
Cambio de recurso 280: Proyecto
Se revisan imágenes del recurso y se actualiza de acuerdo a la solicitud
de Lizzie para que el Proyecto o competencias quede con el estilo
enviado por España.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_MA_08_03_CO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="388">
   <si>
     <t>Asignatura</t>
   </si>
@@ -852,16 +852,10 @@
     <t>Proponer situaciones problema aplicando cocientes notables</t>
   </si>
   <si>
-    <t xml:space="preserve">Proyecto: aplica los productos notables </t>
-  </si>
-  <si>
     <t>Original REC250, tener en cuenta archivo anexo REC205-Generalización1</t>
   </si>
   <si>
     <t>Original REC260</t>
-  </si>
-  <si>
-    <t>Proyecto que propone usar productos notables como modelo matemático de generalización</t>
   </si>
   <si>
     <t>RF</t>
@@ -1328,6 +1322,15 @@
   </si>
   <si>
     <t>Expresiones algebraicas que representan áreas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: aplica los productos notables </t>
+  </si>
+  <si>
+    <t>Actividad que propone usar productos notables como modelo matemático de generalización</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema Identidades notables</t>
   </si>
 </sst>
 </file>
@@ -1742,18 +1745,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1792,6 +1783,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6386,7 +6389,7 @@
   <dimension ref="A1:AR1085"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6420,81 +6423,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="32" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="67" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="71" t="s">
         <v>339</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="G1" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="71" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="75" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>342</v>
-      </c>
-      <c r="I1" s="75" t="s">
+      <c r="I1" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="67" t="s">
-        <v>337</v>
-      </c>
-      <c r="L1" s="66" t="s">
+      <c r="K1" s="63" t="s">
+        <v>335</v>
+      </c>
+      <c r="L1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="M1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="69"/>
+      <c r="N1" s="65"/>
       <c r="O1" s="59" t="s">
         <v>197</v>
       </c>
       <c r="P1" s="59" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q1" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q1" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="S1" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="61" t="s">
+      <c r="T1" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="73" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="66"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="62"/>
       <c r="M2" s="33" t="s">
         <v>124</v>
       </c>
@@ -6503,16 +6506,16 @@
       </c>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="60"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="73"/>
       <c r="W2" s="40" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="X2" s="37" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:44" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -6531,7 +6534,7 @@
       <c r="E3" s="46"/>
       <c r="F3" s="46"/>
       <c r="G3" s="54" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H3" s="46">
         <v>1</v>
@@ -6540,7 +6543,7 @@
         <v>204</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K3" s="42" t="s">
         <v>204</v>
@@ -6555,7 +6558,7 @@
         <v>230</v>
       </c>
       <c r="Q3" s="56" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R3" s="56" t="s">
         <v>262</v>
@@ -6570,10 +6573,10 @@
         <v>267</v>
       </c>
       <c r="V3" s="57" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="W3" s="57" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X3" s="51">
         <v>42294</v>
@@ -6604,7 +6607,7 @@
         <v>205</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>205</v>
@@ -6626,28 +6629,28 @@
         <v>6</v>
       </c>
       <c r="R4" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="S4" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T4" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="U4" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T4" s="48" t="s">
-        <v>293</v>
-      </c>
-      <c r="U4" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V4" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W4" s="57" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X4" s="51">
         <v>42294</v>
       </c>
       <c r="Y4" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
@@ -6677,7 +6680,7 @@
         <v>205</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K5" s="42" t="s">
         <v>205</v>
@@ -6699,22 +6702,22 @@
         <v>6</v>
       </c>
       <c r="R5" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S5" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T5" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="U5" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T5" s="48" t="s">
-        <v>295</v>
-      </c>
-      <c r="U5" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V5" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W5" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X5" s="51">
         <v>42294</v>
@@ -6769,28 +6772,28 @@
         <v>6</v>
       </c>
       <c r="R6" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S6" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T6" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="U6" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T6" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="U6" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V6" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W6" s="41" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="X6" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y6" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:44" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -6850,13 +6853,13 @@
         <v>267</v>
       </c>
       <c r="V7" s="57" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="W7" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X7" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y7" s="35"/>
       <c r="Z7" s="35"/>
@@ -6919,7 +6922,7 @@
         <v>138</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P8" s="47" t="s">
         <v>230</v>
@@ -6928,25 +6931,25 @@
         <v>6</v>
       </c>
       <c r="R8" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S8" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T8" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="U8" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T8" s="48" t="s">
-        <v>297</v>
-      </c>
-      <c r="U8" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V8" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W8" s="50">
         <v>42254</v>
       </c>
       <c r="X8" s="53" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
@@ -6967,7 +6970,7 @@
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="43" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H9" s="46">
         <v>7</v>
@@ -6998,28 +7001,28 @@
         <v>6</v>
       </c>
       <c r="R9" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S9" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T9" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="U9" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T9" s="48" t="s">
-        <v>299</v>
-      </c>
-      <c r="U9" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V9" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W9" s="41" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="X9" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y9" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:44" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -7040,7 +7043,7 @@
       </c>
       <c r="F10" s="45"/>
       <c r="G10" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H10" s="46">
         <v>8</v>
@@ -7049,7 +7052,7 @@
         <v>205</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K10" s="42" t="s">
         <v>204</v>
@@ -7064,28 +7067,28 @@
         <v>230</v>
       </c>
       <c r="Q10" s="56" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="R10" s="56" t="s">
         <v>262</v>
       </c>
       <c r="S10" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="T10" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="U10" s="56" t="s">
         <v>329</v>
       </c>
-      <c r="T10" s="56" t="s">
-        <v>330</v>
-      </c>
-      <c r="U10" s="56" t="s">
-        <v>331</v>
-      </c>
       <c r="V10" s="57" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="W10" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X10" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y10" s="35"/>
       <c r="Z10" s="35"/>
@@ -7126,7 +7129,7 @@
       </c>
       <c r="F11" s="45"/>
       <c r="G11" s="43" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H11" s="46">
         <v>9</v>
@@ -7135,7 +7138,7 @@
         <v>205</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K11" s="42" t="s">
         <v>205</v>
@@ -7157,28 +7160,28 @@
         <v>6</v>
       </c>
       <c r="R11" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S11" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T11" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="U11" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T11" s="48" t="s">
-        <v>300</v>
-      </c>
-      <c r="U11" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V11" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W11" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X11" s="52">
         <v>42294</v>
       </c>
       <c r="Y11" s="30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
@@ -7199,7 +7202,7 @@
       </c>
       <c r="F12" s="45"/>
       <c r="G12" s="43" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H12" s="46">
         <v>10</v>
@@ -7208,7 +7211,7 @@
         <v>204</v>
       </c>
       <c r="J12" s="45" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K12" s="42" t="s">
         <v>205</v>
@@ -7230,28 +7233,28 @@
         <v>6</v>
       </c>
       <c r="R12" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="S12" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T12" s="48" t="s">
         <v>282</v>
       </c>
-      <c r="S12" s="48" t="s">
+      <c r="U12" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T12" s="48" t="s">
-        <v>284</v>
-      </c>
-      <c r="U12" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V12" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W12" s="41" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="X12" s="53">
         <v>42297</v>
       </c>
       <c r="Y12" s="30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -7272,7 +7275,7 @@
       </c>
       <c r="F13" s="45"/>
       <c r="G13" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H13" s="46">
         <v>11</v>
@@ -7303,25 +7306,25 @@
         <v>6</v>
       </c>
       <c r="R13" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S13" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T13" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="U13" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T13" s="48" t="s">
-        <v>301</v>
-      </c>
-      <c r="U13" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V13" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W13" s="35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X13" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
@@ -7373,25 +7376,25 @@
         <v>6</v>
       </c>
       <c r="R14" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S14" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T14" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="U14" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T14" s="48" t="s">
-        <v>302</v>
-      </c>
-      <c r="U14" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V14" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W14" s="35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X14" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
@@ -7443,22 +7446,22 @@
         <v>6</v>
       </c>
       <c r="R15" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S15" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T15" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="U15" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T15" s="48" t="s">
-        <v>303</v>
-      </c>
-      <c r="U15" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V15" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W15" s="41" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="X15" s="53">
         <v>42297</v>
@@ -7513,22 +7516,22 @@
         <v>6</v>
       </c>
       <c r="R16" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S16" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T16" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="U16" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T16" s="48" t="s">
-        <v>286</v>
-      </c>
-      <c r="U16" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V16" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W16" s="41" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X16" s="53">
         <v>42297</v>
@@ -7583,25 +7586,25 @@
         <v>6</v>
       </c>
       <c r="R17" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S17" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T17" s="48" t="s">
+        <v>343</v>
+      </c>
+      <c r="U17" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T17" s="48" t="s">
-        <v>345</v>
-      </c>
-      <c r="U17" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V17" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W17" s="50">
         <v>42292</v>
       </c>
       <c r="X17" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
@@ -7653,25 +7656,25 @@
         <v>6</v>
       </c>
       <c r="R18" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S18" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T18" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="U18" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T18" s="48" t="s">
-        <v>308</v>
-      </c>
-      <c r="U18" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V18" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W18" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X18" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:39" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -7692,7 +7695,7 @@
       </c>
       <c r="F19" s="45"/>
       <c r="G19" s="43" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H19" s="42">
         <v>17</v>
@@ -7701,7 +7704,7 @@
         <v>205</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K19" s="42" t="s">
         <v>204</v>
@@ -7718,28 +7721,28 @@
         <v>230</v>
       </c>
       <c r="Q19" s="56" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="R19" s="56" t="s">
         <v>262</v>
       </c>
       <c r="S19" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="T19" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="U19" s="56" t="s">
         <v>333</v>
       </c>
-      <c r="T19" s="56" t="s">
-        <v>334</v>
-      </c>
-      <c r="U19" s="56" t="s">
-        <v>335</v>
-      </c>
       <c r="V19" s="57" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="W19" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X19" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y19" s="35"/>
       <c r="Z19" s="35"/>
@@ -7774,7 +7777,7 @@
       </c>
       <c r="F20" s="45"/>
       <c r="G20" s="43" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H20" s="42">
         <v>18</v>
@@ -7796,7 +7799,7 @@
         <v>116</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P20" s="47" t="s">
         <v>205</v>
@@ -7805,28 +7808,28 @@
         <v>6</v>
       </c>
       <c r="R20" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S20" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T20" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="U20" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T20" s="48" t="s">
-        <v>298</v>
-      </c>
-      <c r="U20" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V20" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W20" s="41" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X20" s="53">
         <v>42297</v>
       </c>
       <c r="Y20" s="30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
@@ -7876,19 +7879,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S21" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T21" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="U21" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T21" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="U21" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V21" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W21" s="50">
         <v>42297</v>
@@ -7897,7 +7900,7 @@
         <v>42299</v>
       </c>
       <c r="Y21" s="30" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -7949,19 +7952,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S22" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T22" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="U22" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T22" s="48" t="s">
-        <v>290</v>
-      </c>
-      <c r="U22" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V22" s="57" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W22" s="50">
         <v>42294</v>
@@ -8019,28 +8022,28 @@
         <v>6</v>
       </c>
       <c r="R23" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S23" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T23" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="U23" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T23" s="48" t="s">
-        <v>309</v>
-      </c>
-      <c r="U23" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V23" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X23" s="50">
         <v>42297</v>
       </c>
       <c r="Y23" s="30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
@@ -8061,7 +8064,7 @@
       </c>
       <c r="F24" s="45"/>
       <c r="G24" s="43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H24" s="42">
         <v>22</v>
@@ -8092,25 +8095,25 @@
         <v>6</v>
       </c>
       <c r="R24" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S24" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T24" s="48" t="s">
+        <v>302</v>
+      </c>
+      <c r="U24" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T24" s="48" t="s">
-        <v>304</v>
-      </c>
-      <c r="U24" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V24" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W24" s="50">
         <v>42294</v>
       </c>
       <c r="X24" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
@@ -8160,25 +8163,25 @@
         <v>6</v>
       </c>
       <c r="R25" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S25" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T25" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="U25" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T25" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="U25" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V25" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W25" s="50">
         <v>42299</v>
       </c>
       <c r="X25" s="58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
@@ -8197,7 +8200,7 @@
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
       <c r="G26" s="43" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H26" s="46">
         <v>24</v>
@@ -8219,7 +8222,7 @@
         <v>101</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P26" s="47" t="s">
         <v>230</v>
@@ -8228,28 +8231,28 @@
         <v>6</v>
       </c>
       <c r="R26" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S26" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T26" s="48" t="s">
+        <v>341</v>
+      </c>
+      <c r="U26" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T26" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="U26" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V26" s="35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W26" s="41" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="X26" s="58" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Y26" s="30" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -8299,28 +8302,28 @@
         <v>6</v>
       </c>
       <c r="R27" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S27" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="T27" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="U27" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="T27" s="48" t="s">
-        <v>289</v>
-      </c>
-      <c r="U27" s="48" t="s">
-        <v>285</v>
-      </c>
       <c r="V27" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W27" s="41" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X27" s="53">
         <v>42297</v>
       </c>
       <c r="Y27" s="49" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
@@ -8341,7 +8344,7 @@
       </c>
       <c r="F28" s="45"/>
       <c r="G28" s="43" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H28" s="46">
         <v>26</v>
@@ -8350,7 +8353,7 @@
         <v>205</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K28" s="42" t="s">
         <v>205</v>
@@ -8363,7 +8366,7 @@
         <v>116</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="P28" s="47" t="s">
         <v>230</v>
@@ -8372,22 +8375,22 @@
         <v>6</v>
       </c>
       <c r="R28" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S28" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T28" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="U28" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T28" s="48" t="s">
-        <v>305</v>
-      </c>
-      <c r="U28" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V28" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W28" s="41" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="X28" s="53">
         <v>42297</v>
@@ -8411,7 +8414,7 @@
       </c>
       <c r="F29" s="45"/>
       <c r="G29" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H29" s="46">
         <v>27</v>
@@ -8420,7 +8423,7 @@
         <v>205</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K29" s="42" t="s">
         <v>205</v>
@@ -8442,19 +8445,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S29" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T29" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="U29" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T29" s="48" t="s">
-        <v>306</v>
-      </c>
-      <c r="U29" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V29" s="35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W29" s="50">
         <v>42290</v>
@@ -8479,7 +8482,7 @@
       <c r="E30" s="45"/>
       <c r="F30" s="45"/>
       <c r="G30" s="43" t="s">
-        <v>278</v>
+        <v>385</v>
       </c>
       <c r="H30" s="46">
         <v>28</v>
@@ -8488,7 +8491,7 @@
         <v>205</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>281</v>
+        <v>386</v>
       </c>
       <c r="K30" s="42" t="s">
         <v>205</v>
@@ -8501,7 +8504,7 @@
         <v>118</v>
       </c>
       <c r="O30" s="45" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P30" s="47" t="s">
         <v>230</v>
@@ -8510,25 +8513,25 @@
         <v>6</v>
       </c>
       <c r="R30" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S30" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T30" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="U30" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T30" s="48" t="s">
-        <v>307</v>
-      </c>
-      <c r="U30" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V30" s="35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W30" s="50">
         <v>42303</v>
       </c>
       <c r="X30" s="58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:39" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -8547,7 +8550,7 @@
       <c r="E31" s="45"/>
       <c r="F31" s="45"/>
       <c r="G31" s="43" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H31" s="46">
         <v>29</v>
@@ -8590,13 +8593,13 @@
         <v>267</v>
       </c>
       <c r="V31" s="57" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="W31" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X31" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y31" s="35"/>
       <c r="Z31" s="35"/>
@@ -8630,7 +8633,7 @@
       <c r="E32" s="45"/>
       <c r="F32" s="45"/>
       <c r="G32" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H32" s="46">
         <v>30</v>
@@ -8652,7 +8655,7 @@
         <v>138</v>
       </c>
       <c r="O32" s="45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P32" s="47" t="s">
         <v>205</v>
@@ -8661,25 +8664,25 @@
         <v>6</v>
       </c>
       <c r="R32" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S32" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T32" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="U32" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T32" s="48" t="s">
-        <v>311</v>
-      </c>
-      <c r="U32" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V32" s="35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W32" s="50">
         <v>42297</v>
       </c>
       <c r="X32" s="58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Y32" s="35"/>
       <c r="Z32" s="35"/>
@@ -8708,7 +8711,7 @@
         <v>208</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E33" s="45"/>
       <c r="F33" s="45"/>
@@ -8719,7 +8722,9 @@
         <v>31</v>
       </c>
       <c r="I33" s="47"/>
-      <c r="J33" s="45"/>
+      <c r="J33" s="45" t="s">
+        <v>387</v>
+      </c>
       <c r="K33" s="42" t="s">
         <v>205</v>
       </c>
@@ -8735,7 +8740,7 @@
       <c r="U33" s="45"/>
       <c r="V33" s="35"/>
       <c r="W33" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X33" s="53">
         <v>42297</v>
@@ -8752,12 +8757,12 @@
         <v>208</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H34" s="46">
         <v>32</v>
@@ -8766,7 +8771,7 @@
         <v>205</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K34" s="42" t="s">
         <v>205</v>
@@ -8786,25 +8791,25 @@
         <v>6</v>
       </c>
       <c r="R34" s="48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S34" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="T34" s="48" t="s">
+        <v>308</v>
+      </c>
+      <c r="U34" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="T34" s="48" t="s">
-        <v>310</v>
-      </c>
-      <c r="U34" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="V34" s="35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W34" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X34" s="35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
@@ -8818,10 +8823,10 @@
         <v>208</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E35" s="45" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F35" s="45"/>
       <c r="G35" s="43"/>
@@ -8846,7 +8851,7 @@
       <c r="T35" s="45"/>
       <c r="U35" s="45"/>
       <c r="V35" s="35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W35" s="50">
         <v>42296</v>
@@ -8855,7 +8860,7 @@
         <v>42297</v>
       </c>
       <c r="Y35" s="49" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -8918,7 +8923,7 @@
         <v>21</v>
       </c>
       <c r="Q39" s="36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -8934,7 +8939,7 @@
         <v>9</v>
       </c>
       <c r="Q40" s="36" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -12684,6 +12689,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -12698,12 +12709,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K35">

</xml_diff>